<commit_message>
minor update to system impact on failure_mode
</commit_message>
<xml_diff>
--- a/data/inputs/Asset Model.xlsx
+++ b/data/inputs/Asset Model.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mkirton1\OneDrive - KPMG\Documents\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gtreseder\OneDrive - KPMG\Documents\3. Client\Essential Energy\Probability of Failure Model\pof\data\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="253" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{192A1152-185F-4EFB-9237-B5B534F84DAF}"/>
+  <xr:revisionPtr revIDLastSave="256" documentId="13_ncr:1_{9B2AD8C4-B064-4080-85F1-E579881B33AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{A10FE96E-0F64-4A2F-B835-441A8477A789}"/>
   <bookViews>
-    <workbookView xWindow="10452" yWindow="-13068" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="2" r:id="rId1"/>
@@ -3386,7 +3386,7 @@
       <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3400,7 +3400,7 @@
       <selection activeCell="M37" sqref="M37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3414,16 +3414,16 @@
       <selection activeCell="A72" sqref="A72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="7" max="8" width="10.6640625" customWidth="1"/>
-    <col min="13" max="13" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="32.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="7" max="8" width="10.7109375" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>260</v>
       </c>
@@ -3431,7 +3431,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>262</v>
       </c>
@@ -3439,7 +3439,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>264</v>
       </c>
@@ -3447,17 +3447,17 @@
         <v>265</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O12" s="1" t="s">
         <v>187</v>
       </c>
@@ -3468,7 +3468,7 @@
         <v>269</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F13" s="1" t="s">
         <v>270</v>
       </c>
@@ -3482,7 +3482,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F14" s="12" t="s">
         <v>273</v>
       </c>
@@ -3496,7 +3496,7 @@
         <v>275</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F15" t="s">
         <v>276</v>
       </c>
@@ -3513,7 +3513,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
         <v>280</v>
       </c>
@@ -3524,7 +3524,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F17" t="s">
         <v>282</v>
       </c>
@@ -3535,22 +3535,22 @@
         <v>284</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="O18" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="F20" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
         <v>288</v>
       </c>
@@ -3576,7 +3576,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>203</v>
       </c>
@@ -3590,7 +3590,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="33" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:19" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>187</v>
       </c>
@@ -3604,7 +3604,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C34" t="s">
         <v>271</v>
       </c>
@@ -3618,7 +3618,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="35" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C35" t="s">
         <v>278</v>
       </c>
@@ -3638,7 +3638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D36" t="s">
         <v>291</v>
       </c>
@@ -3652,7 +3652,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:19" x14ac:dyDescent="0.25">
       <c r="D37" s="43" t="s">
         <v>18</v>
       </c>
@@ -3660,7 +3660,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="38" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C38" t="s">
         <v>285</v>
       </c>
@@ -3671,7 +3671,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:19" x14ac:dyDescent="0.25">
       <c r="C39" t="s">
         <v>271</v>
       </c>
@@ -3682,27 +3682,27 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K40" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="41" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K41" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="42" spans="2:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:19" x14ac:dyDescent="0.25">
       <c r="K42" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="H52" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
         <v>294</v>
       </c>
@@ -3719,7 +3719,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E54" s="1" t="s">
         <v>296</v>
       </c>
@@ -3747,23 +3747,23 @@
         <v>28800</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="L55">
         <f>L54/60/60</f>
         <v>8</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F59" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
         <v>299</v>
       </c>
@@ -3771,17 +3771,17 @@
         <v>96</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E61" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E62" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B65" t="s">
         <v>107</v>
       </c>
@@ -3789,12 +3789,12 @@
         <v>302</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>304</v>
       </c>
@@ -3805,7 +3805,7 @@
         <v>305</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>306</v>
       </c>
@@ -3816,7 +3816,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>308</v>
       </c>
@@ -3829,7 +3829,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="O13:O15 O17:O18">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3846,20 +3846,20 @@
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P3" s="1"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1" t="s">
@@ -3869,7 +3869,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>313</v>
       </c>
@@ -3892,7 +3892,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>316</v>
       </c>
@@ -3916,7 +3916,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H6" t="s">
         <v>320</v>
       </c>
@@ -3939,7 +3939,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="P7" s="1"/>
       <c r="Q7" s="1" t="s">
         <v>322</v>
@@ -3951,7 +3951,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H8" t="s">
         <v>321</v>
       </c>
@@ -3969,7 +3969,7 @@
         <v>315</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>324</v>
       </c>
@@ -3980,7 +3980,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="H10" t="s">
         <v>323</v>
       </c>
@@ -3988,12 +3988,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>325</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>295</v>
       </c>
@@ -4005,7 +4005,7 @@
         <v>7.4</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="J16" t="s">
         <v>326</v>
       </c>
@@ -4013,12 +4013,12 @@
         <v>327</v>
       </c>
     </row>
-    <row r="19" spans="10:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="10:10" x14ac:dyDescent="0.25">
       <c r="J19" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="1048576" spans="15:15" x14ac:dyDescent="0.3">
+    <row r="1048576" spans="15:15" x14ac:dyDescent="0.25">
       <c r="O1048576" t="s">
         <v>315</v>
       </c>
@@ -4037,34 +4037,34 @@
       <selection activeCell="D4" sqref="D4:AC4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="12.6640625" customWidth="1"/>
-    <col min="12" max="12" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.109375" customWidth="1"/>
-    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.6640625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" customWidth="1"/>
+    <col min="18" max="18" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="12" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13.6640625" customWidth="1"/>
-    <col min="26" max="26" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="27" max="27" width="12" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.33203125" customWidth="1"/>
-    <col min="31" max="31" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.28515625" customWidth="1"/>
+    <col min="31" max="31" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4105,7 +4105,7 @@
       </c>
       <c r="AA1" s="1"/>
     </row>
-    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
         <v>6</v>
       </c>
@@ -4192,7 +4192,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>28</v>
       </c>
@@ -4273,7 +4273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="L4" s="3" t="s">
         <v>38</v>
       </c>
@@ -4299,62 +4299,62 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEA0734F-FFBE-4DAF-BDE5-A12359370A0D}">
   <dimension ref="A1:BA78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AI1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AU16" sqref="AU16"/>
+      <selection pane="bottomLeft" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.109375" customWidth="1" outlineLevel="1"/>
-    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1" outlineLevel="1"/>
-    <col min="3" max="3" width="13.109375" customWidth="1" outlineLevel="1"/>
-    <col min="4" max="4" width="13.109375" customWidth="1"/>
-    <col min="5" max="5" width="13.109375" style="77" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
-    <col min="7" max="9" width="13.109375" customWidth="1"/>
-    <col min="10" max="10" width="23.44140625" customWidth="1"/>
-    <col min="11" max="11" width="6.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.6640625" customWidth="1"/>
-    <col min="13" max="13" width="13.88671875" customWidth="1"/>
-    <col min="14" max="14" width="8.88671875" customWidth="1"/>
-    <col min="15" max="15" width="12.109375" style="112" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" customWidth="1" outlineLevel="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1" outlineLevel="1"/>
+    <col min="3" max="3" width="13.140625" customWidth="1" outlineLevel="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="77" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="9" width="13.140625" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" customWidth="1"/>
+    <col min="11" max="11" width="6.28515625" customWidth="1"/>
+    <col min="12" max="12" width="11.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.85546875" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" style="112" customWidth="1"/>
     <col min="16" max="16" width="6" style="114" customWidth="1"/>
-    <col min="17" max="17" width="14.44140625" customWidth="1"/>
-    <col min="18" max="18" width="6.88671875" customWidth="1"/>
-    <col min="19" max="19" width="9.6640625" style="100" customWidth="1"/>
-    <col min="20" max="20" width="25.6640625" customWidth="1"/>
-    <col min="21" max="21" width="8.88671875" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
-    <col min="23" max="23" width="6.6640625" style="77" customWidth="1"/>
-    <col min="24" max="24" width="23.5546875" customWidth="1"/>
-    <col min="25" max="25" width="6.33203125" customWidth="1"/>
-    <col min="26" max="26" width="11.109375" customWidth="1"/>
-    <col min="27" max="27" width="8.88671875" customWidth="1"/>
-    <col min="28" max="28" width="14.88671875" customWidth="1"/>
-    <col min="29" max="29" width="10.33203125" customWidth="1"/>
-    <col min="30" max="30" width="14.88671875" customWidth="1"/>
-    <col min="31" max="31" width="14.6640625" customWidth="1"/>
-    <col min="32" max="32" width="8.88671875" customWidth="1"/>
-    <col min="33" max="33" width="9.5546875" customWidth="1"/>
-    <col min="34" max="34" width="23.5546875" style="77" customWidth="1"/>
+    <col min="17" max="17" width="14.42578125" customWidth="1"/>
+    <col min="18" max="18" width="6.85546875" customWidth="1"/>
+    <col min="19" max="19" width="9.7109375" style="100" customWidth="1"/>
+    <col min="20" max="20" width="25.7109375" customWidth="1"/>
+    <col min="21" max="21" width="8.85546875" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
+    <col min="23" max="23" width="6.7109375" style="77" customWidth="1"/>
+    <col min="24" max="24" width="23.5703125" customWidth="1"/>
+    <col min="25" max="25" width="6.28515625" customWidth="1"/>
+    <col min="26" max="26" width="11.140625" customWidth="1"/>
+    <col min="27" max="27" width="8.85546875" customWidth="1"/>
+    <col min="28" max="28" width="14.85546875" customWidth="1"/>
+    <col min="29" max="29" width="10.28515625" customWidth="1"/>
+    <col min="30" max="30" width="14.85546875" customWidth="1"/>
+    <col min="31" max="31" width="14.7109375" customWidth="1"/>
+    <col min="32" max="32" width="8.85546875" customWidth="1"/>
+    <col min="33" max="33" width="9.5703125" customWidth="1"/>
+    <col min="34" max="34" width="23.5703125" style="77" customWidth="1"/>
     <col min="35" max="35" width="12" customWidth="1"/>
-    <col min="36" max="37" width="11.5546875" customWidth="1"/>
-    <col min="38" max="41" width="8.88671875" style="17" customWidth="1"/>
-    <col min="42" max="42" width="8.88671875" style="86" customWidth="1"/>
-    <col min="43" max="43" width="17.88671875" style="71" customWidth="1"/>
-    <col min="44" max="44" width="14.109375" style="20" customWidth="1"/>
-    <col min="45" max="45" width="14.44140625" style="92" customWidth="1"/>
-    <col min="46" max="47" width="8.88671875" style="17" customWidth="1"/>
-    <col min="48" max="48" width="8.88671875" style="86" customWidth="1"/>
-    <col min="49" max="49" width="17.88671875" customWidth="1"/>
-    <col min="50" max="50" width="8.88671875" style="20" customWidth="1"/>
-    <col min="51" max="51" width="16.33203125" customWidth="1"/>
-    <col min="52" max="52" width="8.88671875" customWidth="1"/>
-    <col min="53" max="53" width="16.109375" style="17" bestFit="1" customWidth="1"/>
+    <col min="36" max="37" width="11.5703125" customWidth="1"/>
+    <col min="38" max="41" width="8.85546875" style="17" customWidth="1"/>
+    <col min="42" max="42" width="8.85546875" style="86" customWidth="1"/>
+    <col min="43" max="43" width="17.85546875" style="71" customWidth="1"/>
+    <col min="44" max="44" width="14.140625" style="20" customWidth="1"/>
+    <col min="45" max="45" width="14.42578125" style="92" customWidth="1"/>
+    <col min="46" max="47" width="8.85546875" style="17" customWidth="1"/>
+    <col min="48" max="48" width="8.85546875" style="86" customWidth="1"/>
+    <col min="49" max="49" width="17.85546875" customWidth="1"/>
+    <col min="50" max="50" width="8.85546875" style="20" customWidth="1"/>
+    <col min="51" max="51" width="16.28515625" customWidth="1"/>
+    <col min="52" max="52" width="8.85546875" customWidth="1"/>
+    <col min="53" max="53" width="16.140625" style="17" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>39</v>
@@ -4423,7 +4423,7 @@
       <c r="AZ1" s="64"/>
       <c r="BA1" s="21"/>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>45</v>
@@ -4512,7 +4512,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>55</v>
       </c>
@@ -4673,7 +4673,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="59"/>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
@@ -4728,7 +4728,7 @@
       <c r="AZ4" s="59"/>
       <c r="BA4" s="61"/>
     </row>
-    <row r="5" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B5" s="145" t="s">
         <v>331</v>
       </c>
@@ -4842,7 +4842,7 @@
       <c r="AY5" s="17"/>
       <c r="AZ5" s="17"/>
     </row>
-    <row r="6" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:53" x14ac:dyDescent="0.25">
       <c r="F6" t="s">
         <v>38</v>
       </c>
@@ -4876,7 +4876,7 @@
       <c r="AY6" s="17"/>
       <c r="AZ6" s="17"/>
     </row>
-    <row r="7" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:53" x14ac:dyDescent="0.25">
       <c r="F7" t="s">
         <v>37</v>
       </c>
@@ -4920,7 +4920,7 @@
       <c r="AZ7" s="65"/>
       <c r="BA7" s="66"/>
     </row>
-    <row r="8" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X8" t="s">
         <v>89</v>
       </c>
@@ -4988,7 +4988,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AQ9" s="70" t="s">
         <v>38</v>
       </c>
@@ -5011,7 +5011,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X10" s="65"/>
       <c r="Y10" s="65"/>
       <c r="Z10" s="65"/>
@@ -5043,7 +5043,7 @@
       <c r="AZ10" s="65"/>
       <c r="BA10" s="66"/>
     </row>
-    <row r="11" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X11" t="s">
         <v>95</v>
       </c>
@@ -5111,7 +5111,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X12" s="65"/>
       <c r="Y12" s="65"/>
       <c r="Z12" s="65"/>
@@ -5143,7 +5143,7 @@
       <c r="AZ12" s="65"/>
       <c r="BA12" s="66"/>
     </row>
-    <row r="13" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X13" t="s">
         <v>98</v>
       </c>
@@ -5202,7 +5202,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J14" s="123"/>
       <c r="K14" s="123"/>
       <c r="L14" s="123"/>
@@ -5248,12 +5248,12 @@
       <c r="AZ14" s="123"/>
       <c r="BA14" s="128"/>
     </row>
-    <row r="15" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:53" x14ac:dyDescent="0.25">
       <c r="J15" t="s">
         <v>99</v>
       </c>
       <c r="K15">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L15" s="45" t="s">
         <v>79</v>
@@ -5293,7 +5293,7 @@
         <v>0.96</v>
       </c>
       <c r="AA15">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="AB15" t="s">
         <v>51</v>
@@ -5333,7 +5333,7 @@
       <c r="AY15" s="17"/>
       <c r="AZ15" s="17"/>
     </row>
-    <row r="16" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X16" s="65"/>
       <c r="Y16" s="65"/>
       <c r="Z16" s="65"/>
@@ -5365,7 +5365,7 @@
       <c r="AZ16" s="65"/>
       <c r="BA16" s="66"/>
     </row>
-    <row r="17" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="17" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X17" t="s">
         <v>95</v>
       </c>
@@ -5433,7 +5433,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="18" spans="10:53" x14ac:dyDescent="0.25">
       <c r="AL18"/>
       <c r="AM18"/>
       <c r="AN18"/>
@@ -5449,7 +5449,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="19" spans="10:53" x14ac:dyDescent="0.25">
       <c r="AQ19" s="71" t="s">
         <v>37</v>
       </c>
@@ -5460,7 +5460,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="20" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X20" s="65"/>
       <c r="Y20" s="65"/>
       <c r="Z20" s="65"/>
@@ -5492,7 +5492,7 @@
       <c r="AZ20" s="65"/>
       <c r="BA20" s="66"/>
     </row>
-    <row r="21" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="21" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X21" t="s">
         <v>98</v>
       </c>
@@ -5548,7 +5548,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="22" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J22" s="123"/>
       <c r="K22" s="123"/>
       <c r="L22" s="123"/>
@@ -5594,12 +5594,12 @@
       <c r="AZ22" s="123"/>
       <c r="BA22" s="128"/>
     </row>
-    <row r="23" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="23" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J23" t="s">
         <v>100</v>
       </c>
       <c r="K23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L23" s="45" t="s">
         <v>79</v>
@@ -5682,7 +5682,7 @@
       <c r="AY23" s="17"/>
       <c r="AZ23" s="17"/>
     </row>
-    <row r="24" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="24" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X24" s="65"/>
       <c r="Y24" s="65"/>
       <c r="Z24" s="65"/>
@@ -5714,7 +5714,7 @@
       <c r="AZ24" s="65"/>
       <c r="BA24" s="66"/>
     </row>
-    <row r="25" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="25" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X25" t="s">
         <v>101</v>
       </c>
@@ -5782,7 +5782,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="26" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="26" spans="10:53" x14ac:dyDescent="0.25">
       <c r="AQ26" s="70" t="s">
         <v>38</v>
       </c>
@@ -5793,7 +5793,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="27" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="27" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X27" s="65"/>
       <c r="Y27" s="65"/>
       <c r="Z27" s="65"/>
@@ -5825,7 +5825,7 @@
       <c r="AZ27" s="65"/>
       <c r="BA27" s="66"/>
     </row>
-    <row r="28" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="28" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X28" t="s">
         <v>95</v>
       </c>
@@ -5893,14 +5893,14 @@
         <v>45</v>
       </c>
     </row>
-    <row r="29" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="29" spans="10:53" x14ac:dyDescent="0.25">
       <c r="AL29"/>
       <c r="AM29"/>
       <c r="AN29"/>
       <c r="AO29"/>
       <c r="AP29" s="77"/>
     </row>
-    <row r="31" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="31" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X31" s="65"/>
       <c r="Y31" s="65"/>
       <c r="Z31" s="65"/>
@@ -5932,7 +5932,7 @@
       <c r="AZ31" s="65"/>
       <c r="BA31" s="66"/>
     </row>
-    <row r="32" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="32" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X32" t="s">
         <v>98</v>
       </c>
@@ -5988,7 +5988,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="33" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="33" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J33" s="123"/>
       <c r="K33" s="123"/>
       <c r="L33" s="123"/>
@@ -6034,7 +6034,7 @@
       <c r="AZ33" s="123"/>
       <c r="BA33" s="128"/>
     </row>
-    <row r="34" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="34" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J34" t="s">
         <v>102</v>
       </c>
@@ -6109,7 +6109,7 @@
       </c>
       <c r="AV34" s="105"/>
     </row>
-    <row r="35" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="35" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X35" s="65"/>
       <c r="Y35" s="65"/>
       <c r="Z35" s="65"/>
@@ -6141,7 +6141,7 @@
       <c r="AZ35" s="65"/>
       <c r="BA35" s="66"/>
     </row>
-    <row r="36" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="36" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X36" t="s">
         <v>104</v>
       </c>
@@ -6192,7 +6192,7 @@
       <c r="AY36" s="17"/>
       <c r="AZ36" s="17"/>
     </row>
-    <row r="37" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="37" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X37" s="65"/>
       <c r="Y37" s="65"/>
       <c r="Z37" s="65"/>
@@ -6224,7 +6224,7 @@
       <c r="AZ37" s="65"/>
       <c r="BA37" s="66"/>
     </row>
-    <row r="38" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="38" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X38" t="s">
         <v>98</v>
       </c>
@@ -6280,7 +6280,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="39" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="39" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J39" s="123"/>
       <c r="K39" s="123"/>
       <c r="L39" s="123"/>
@@ -6326,7 +6326,7 @@
       <c r="AZ39" s="123"/>
       <c r="BA39" s="128"/>
     </row>
-    <row r="40" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="40" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J40" t="s">
         <v>106</v>
       </c>
@@ -6395,7 +6395,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="41" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X41" s="65"/>
       <c r="Y41" s="65"/>
       <c r="Z41" s="65"/>
@@ -6427,7 +6427,7 @@
       <c r="AZ41" s="65"/>
       <c r="BA41" s="66"/>
     </row>
-    <row r="42" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="42" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X42" t="s">
         <v>98</v>
       </c>
@@ -6483,7 +6483,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="43" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J43" s="123"/>
       <c r="K43" s="123"/>
       <c r="L43" s="123"/>
@@ -6529,7 +6529,7 @@
       <c r="AZ43" s="123"/>
       <c r="BA43" s="128"/>
     </row>
-    <row r="44" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="44" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J44" t="s">
         <v>107</v>
       </c>
@@ -6598,7 +6598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="45" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X45" s="65"/>
       <c r="Y45" s="65"/>
       <c r="Z45" s="65"/>
@@ -6630,7 +6630,7 @@
       <c r="AZ45" s="65"/>
       <c r="BA45" s="66"/>
     </row>
-    <row r="46" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="46" spans="10:53" x14ac:dyDescent="0.25">
       <c r="X46" t="s">
         <v>98</v>
       </c>
@@ -6686,7 +6686,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="47" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="47" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J47" s="123"/>
       <c r="K47" s="123"/>
       <c r="L47" s="123"/>
@@ -6732,7 +6732,7 @@
       <c r="AZ47" s="123"/>
       <c r="BA47" s="128"/>
     </row>
-    <row r="48" spans="10:53" x14ac:dyDescent="0.3">
+    <row r="48" spans="10:53" x14ac:dyDescent="0.25">
       <c r="J48" t="s">
         <v>108</v>
       </c>
@@ -6813,7 +6813,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:53" x14ac:dyDescent="0.25">
       <c r="T49" t="s">
         <v>38</v>
       </c>
@@ -6851,7 +6851,7 @@
       <c r="AZ49" s="65"/>
       <c r="BA49" s="66"/>
     </row>
-    <row r="50" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:53" x14ac:dyDescent="0.25">
       <c r="D50" s="107"/>
       <c r="E50" s="78"/>
       <c r="X50" t="s">
@@ -6921,7 +6921,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="51" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AL51"/>
       <c r="AM51"/>
       <c r="AN51"/>
@@ -6937,7 +6937,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="52" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AQ52" s="71" t="s">
         <v>37</v>
       </c>
@@ -6948,7 +6948,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="53" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X53" s="65"/>
       <c r="Y53" s="65"/>
       <c r="Z53" s="65"/>
@@ -6980,7 +6980,7 @@
       <c r="AZ53" s="65"/>
       <c r="BA53" s="66"/>
     </row>
-    <row r="54" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X54" t="s">
         <v>98</v>
       </c>
@@ -7033,7 +7033,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="55" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="59"/>
       <c r="B55" s="59"/>
       <c r="C55" s="59"/>
@@ -7088,7 +7088,7 @@
       <c r="AZ55" s="59"/>
       <c r="BA55" s="61"/>
     </row>
-    <row r="56" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B56" s="145" t="s">
         <v>343</v>
       </c>
@@ -7189,7 +7189,7 @@
       <c r="AY56" s="17"/>
       <c r="AZ56" s="17"/>
     </row>
-    <row r="57" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C57" s="41"/>
       <c r="D57" s="107"/>
       <c r="E57" s="78"/>
@@ -7224,7 +7224,7 @@
       <c r="AZ57" s="65"/>
       <c r="BA57" s="66"/>
     </row>
-    <row r="58" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X58" t="s">
         <v>95</v>
       </c>
@@ -7292,7 +7292,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="59" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AL59"/>
       <c r="AM59"/>
       <c r="AN59"/>
@@ -7308,7 +7308,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="60" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AQ60" s="71" t="s">
         <v>37</v>
       </c>
@@ -7319,7 +7319,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="61" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X61" s="65"/>
       <c r="Y61" s="65"/>
       <c r="Z61" s="65"/>
@@ -7351,7 +7351,7 @@
       <c r="AZ61" s="65"/>
       <c r="BA61" s="66"/>
     </row>
-    <row r="62" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X62" t="s">
         <v>98</v>
       </c>
@@ -7404,7 +7404,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="63" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:53" ht="12" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="59"/>
       <c r="B63" s="59"/>
       <c r="C63" s="59"/>
@@ -7459,7 +7459,7 @@
       <c r="AZ63" s="59"/>
       <c r="BA63" s="61"/>
     </row>
-    <row r="64" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B64" s="145" t="s">
         <v>331</v>
       </c>
@@ -7566,7 +7566,7 @@
       <c r="AY64" s="17"/>
       <c r="AZ64" s="17"/>
     </row>
-    <row r="65" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:53" x14ac:dyDescent="0.25">
       <c r="C65" s="41"/>
       <c r="D65" s="107"/>
       <c r="E65" s="78"/>
@@ -7620,7 +7620,7 @@
       <c r="AZ65" s="65"/>
       <c r="BA65" s="66"/>
     </row>
-    <row r="66" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:53" x14ac:dyDescent="0.25">
       <c r="F66" t="s">
         <v>37</v>
       </c>
@@ -7700,7 +7700,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AL67"/>
       <c r="AM67"/>
       <c r="AN67"/>
@@ -7716,7 +7716,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="68" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AQ68" s="71" t="s">
         <v>37</v>
       </c>
@@ -7727,7 +7727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="69" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X69" s="65"/>
       <c r="Y69" s="65"/>
       <c r="Z69" s="65"/>
@@ -7759,7 +7759,7 @@
       <c r="AZ69" s="65"/>
       <c r="BA69" s="66"/>
     </row>
-    <row r="70" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X70" t="s">
         <v>98</v>
       </c>
@@ -7812,7 +7812,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="71" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:53" x14ac:dyDescent="0.25">
       <c r="A71" s="136"/>
       <c r="B71" s="136"/>
       <c r="C71" s="136"/>
@@ -7867,7 +7867,7 @@
       <c r="AZ71" s="136"/>
       <c r="BA71" s="140"/>
     </row>
-    <row r="72" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B72" s="145" t="s">
         <v>331</v>
       </c>
@@ -7972,7 +7972,7 @@
       <c r="AY72" s="17"/>
       <c r="AZ72" s="17"/>
     </row>
-    <row r="73" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:53" x14ac:dyDescent="0.25">
       <c r="F73" t="s">
         <v>38</v>
       </c>
@@ -8023,7 +8023,7 @@
       <c r="AZ73" s="65"/>
       <c r="BA73" s="66"/>
     </row>
-    <row r="74" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:53" x14ac:dyDescent="0.25">
       <c r="F74" t="s">
         <v>37</v>
       </c>
@@ -8103,7 +8103,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="75" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AL75"/>
       <c r="AM75"/>
       <c r="AN75"/>
@@ -8119,7 +8119,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="76" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:53" x14ac:dyDescent="0.25">
       <c r="AQ76" s="71" t="s">
         <v>37</v>
       </c>
@@ -8130,7 +8130,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="77" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:53" x14ac:dyDescent="0.25">
       <c r="X77" s="65"/>
       <c r="Y77" s="65"/>
       <c r="Z77" s="65"/>
@@ -8162,7 +8162,7 @@
       <c r="AZ77" s="65"/>
       <c r="BA77" s="66"/>
     </row>
-    <row r="78" spans="1:53" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:53" x14ac:dyDescent="0.25">
       <c r="B78" s="1"/>
       <c r="C78" s="1"/>
       <c r="D78" s="1"/>
@@ -8850,67 +8850,67 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA74">
-    <cfRule type="cellIs" dxfId="12" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="13" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA66">
-    <cfRule type="cellIs" dxfId="11" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA62">
-    <cfRule type="cellIs" dxfId="10" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA58">
-    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="17" priority="10" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA54">
-    <cfRule type="cellIs" dxfId="8" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="16" priority="9" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA50">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA46">
-    <cfRule type="cellIs" dxfId="6" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA32">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="13" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA28">
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="12" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA21">
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA17">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA13">
-    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BA11">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8928,14 +8928,14 @@
       <selection activeCell="N16" sqref="N16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="20" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="J2" s="1"/>
       <c r="Q2" s="26" t="s">
         <v>119</v>
@@ -8950,7 +8950,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B3" s="1" t="s">
         <v>119</v>
       </c>
@@ -8959,7 +8959,7 @@
       </c>
       <c r="Q3" s="28"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>337</v>
       </c>
@@ -8976,7 +8976,7 @@
       <c r="S4" s="29"/>
       <c r="T4" s="29"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>127</v>
       </c>
@@ -8987,7 +8987,7 @@
       <c r="S5" s="29"/>
       <c r="T5" s="29"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C6" t="s">
         <v>128</v>
       </c>
@@ -8998,7 +8998,7 @@
       </c>
       <c r="T6" s="31"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C7" t="s">
         <v>129</v>
       </c>
@@ -9006,7 +9006,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>332</v>
       </c>
@@ -9017,7 +9017,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C9" t="s">
         <v>334</v>
       </c>
@@ -9025,7 +9025,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C10" t="s">
         <v>335</v>
       </c>
@@ -9033,7 +9033,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
         <v>336</v>
       </c>
@@ -9041,7 +9041,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="Q12" s="31"/>
       <c r="R12" s="31"/>
       <c r="S12" s="31" t="s">
@@ -9049,12 +9049,12 @@
       </c>
       <c r="T12" s="31"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="T13" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>338</v>
       </c>
@@ -9071,7 +9071,7 @@
       </c>
       <c r="T14" s="31"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>341</v>
       </c>
@@ -9079,7 +9079,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>334</v>
       </c>
@@ -9093,7 +9093,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>333</v>
       </c>
@@ -9101,7 +9101,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
         <v>339</v>
       </c>
@@ -9112,7 +9112,7 @@
       <c r="S18" s="29"/>
       <c r="T18" s="29"/>
     </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B19" t="s">
         <v>336</v>
       </c>
@@ -9123,78 +9123,78 @@
       </c>
       <c r="T19" s="31"/>
     </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:20" x14ac:dyDescent="0.25">
       <c r="T20" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q21" s="28"/>
       <c r="S21" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q22" s="28"/>
       <c r="T22" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q23" s="28"/>
       <c r="S23" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q24" s="28"/>
       <c r="T24" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q25" s="28"/>
       <c r="T25" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="26" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q26" s="28"/>
       <c r="S26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="27" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q27" s="28"/>
       <c r="S27" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q28" s="28"/>
       <c r="T28" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q29" s="28"/>
       <c r="S29" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="30" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q30" s="28"/>
       <c r="T30" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q31" s="28"/>
       <c r="T31" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="2:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:20" x14ac:dyDescent="0.25">
       <c r="Q32" s="29"/>
       <c r="R32" s="30" t="s">
         <v>150</v>
@@ -9202,7 +9202,7 @@
       <c r="S32" s="29"/>
       <c r="T32" s="29"/>
     </row>
-    <row r="33" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="33" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q33" s="31"/>
       <c r="R33" s="31"/>
       <c r="S33" s="31" t="s">
@@ -9210,13 +9210,13 @@
       </c>
       <c r="T33" s="31"/>
     </row>
-    <row r="34" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="34" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q34" s="28"/>
       <c r="T34" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q35" s="31"/>
       <c r="R35" s="31"/>
       <c r="S35" s="31" t="s">
@@ -9224,13 +9224,13 @@
       </c>
       <c r="T35" s="31"/>
     </row>
-    <row r="36" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="36" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q36" s="28"/>
       <c r="T36" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="37" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="37" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q37" s="29"/>
       <c r="R37" s="30" t="s">
         <v>154</v>
@@ -9238,7 +9238,7 @@
       <c r="S37" s="29"/>
       <c r="T37" s="29"/>
     </row>
-    <row r="38" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q38" s="31"/>
       <c r="R38" s="31"/>
       <c r="S38" s="31" t="s">
@@ -9246,13 +9246,13 @@
       </c>
       <c r="T38" s="31"/>
     </row>
-    <row r="39" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q39" s="28"/>
       <c r="T39" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="40" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q40" s="31"/>
       <c r="R40" s="31"/>
       <c r="S40" s="31" t="s">
@@ -9260,7 +9260,7 @@
       </c>
       <c r="T40" s="31"/>
     </row>
-    <row r="41" spans="17:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="17:20" x14ac:dyDescent="0.25">
       <c r="Q41" s="28"/>
       <c r="T41" t="s">
         <v>157</v>
@@ -9280,20 +9280,20 @@
       <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="12.6640625" customWidth="1"/>
-    <col min="6" max="6" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.33203125" customWidth="1"/>
-    <col min="11" max="11" width="6.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.28515625" customWidth="1"/>
+    <col min="11" max="11" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="9" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
@@ -9307,7 +9307,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>9</v>
       </c>
@@ -9333,7 +9333,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>160</v>
       </c>
@@ -9359,7 +9359,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
         <v>79</v>
       </c>
@@ -9373,7 +9373,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>161</v>
       </c>
@@ -9390,7 +9390,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>163</v>
       </c>
@@ -9410,7 +9410,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>164</v>
       </c>
@@ -9421,7 +9421,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>165</v>
       </c>
@@ -9447,7 +9447,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>166</v>
       </c>
@@ -9458,7 +9458,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>167</v>
       </c>
@@ -9469,7 +9469,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>168</v>
       </c>
@@ -9477,7 +9477,7 @@
       <c r="C11" s="42"/>
       <c r="D11" s="42"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>169</v>
       </c>
@@ -9504,7 +9504,7 @@
       </c>
       <c r="J12" s="45"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>171</v>
       </c>
@@ -9512,22 +9512,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="42" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>175</v>
       </c>
@@ -9547,7 +9547,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>175</v>
       </c>
@@ -9581,14 +9581,14 @@
       <selection activeCell="A2" sqref="A2:G11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>123</v>
       </c>
@@ -9605,7 +9605,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -9619,7 +9619,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>38</v>
       </c>
@@ -9630,7 +9630,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>177</v>
       </c>
@@ -9647,7 +9647,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>180</v>
       </c>
@@ -9661,7 +9661,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>183</v>
       </c>
@@ -9669,7 +9669,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>184</v>
       </c>
@@ -9677,7 +9677,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>185</v>
       </c>
@@ -9688,7 +9688,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B10" s="3" t="s">
         <v>186</v>
       </c>
@@ -9713,33 +9713,33 @@
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="13.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
+    <col min="1" max="2" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="17" max="21" width="9.109375" style="17"/>
-    <col min="22" max="22" width="2.88671875" style="51" customWidth="1"/>
-    <col min="23" max="23" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="14.109375" style="20" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="14.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="2.44140625" style="54" customWidth="1"/>
-    <col min="27" max="29" width="9.109375" style="17"/>
-    <col min="30" max="30" width="2.44140625" style="51" customWidth="1"/>
-    <col min="31" max="31" width="17.88671875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="2.44140625" style="48" customWidth="1"/>
+    <col min="15" max="16" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="21" width="9.140625" style="17"/>
+    <col min="22" max="22" width="2.85546875" style="51" customWidth="1"/>
+    <col min="23" max="23" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.140625" style="20" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="14.42578125" style="20" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="2.42578125" style="54" customWidth="1"/>
+    <col min="27" max="29" width="9.140625" style="17"/>
+    <col min="30" max="30" width="2.42578125" style="51" customWidth="1"/>
+    <col min="31" max="31" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.85546875" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="2.42578125" style="48" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="E1" s="25"/>
       <c r="F1" s="25"/>
       <c r="G1" s="25"/>
@@ -9776,7 +9776,7 @@
       <c r="AH1" s="4"/>
       <c r="AI1" s="46"/>
     </row>
-    <row r="2" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>188</v>
       </c>
@@ -9826,7 +9826,7 @@
       <c r="AH2" s="4"/>
       <c r="AI2" s="46"/>
     </row>
-    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -9922,7 +9922,7 @@
       </c>
       <c r="AI3" s="46"/>
     </row>
-    <row r="4" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>28</v>
       </c>
@@ -9994,7 +9994,7 @@
       <c r="AH4" s="18"/>
       <c r="AI4" s="47"/>
     </row>
-    <row r="5" spans="1:35" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:35" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
       <c r="B5" s="15"/>
       <c r="Q5" s="50"/>
@@ -10015,7 +10015,7 @@
       <c r="AG5" s="50"/>
       <c r="AH5" s="50"/>
     </row>
-    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C6" s="15" t="s">
         <v>195</v>
       </c>
@@ -10075,7 +10075,7 @@
       <c r="AH6" s="18"/>
       <c r="AI6" s="47"/>
     </row>
-    <row r="7" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="S7" s="16"/>
@@ -10104,7 +10104,7 @@
       <c r="AD7" s="50"/>
       <c r="AI7" s="47"/>
     </row>
-    <row r="8" spans="1:35" s="47" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:35" s="47" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="15"/>
       <c r="B8" s="15"/>
       <c r="Q8" s="50"/>
@@ -10121,7 +10121,7 @@
       <c r="AC8" s="50"/>
       <c r="AD8" s="50"/>
     </row>
-    <row r="9" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C9" s="15" t="s">
         <v>197</v>
       </c>
@@ -10189,7 +10189,7 @@
       </c>
       <c r="AI9" s="47"/>
     </row>
-    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="V10" s="47"/>
       <c r="W10" s="15" t="s">
         <v>38</v>
@@ -10207,7 +10207,7 @@
       <c r="AD10" s="50"/>
       <c r="AI10" s="47"/>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
       <c r="W11" s="15" t="s">
         <v>37</v>
       </c>
@@ -10218,7 +10218,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="S12" s="16"/>
@@ -10234,7 +10234,7 @@
       <c r="AD12" s="50"/>
       <c r="AI12" s="47"/>
     </row>
-    <row r="13" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="S13" s="16"/>
@@ -10250,7 +10250,7 @@
       <c r="AD13" s="50"/>
       <c r="AI13" s="47"/>
     </row>
-    <row r="14" spans="1:35" s="56" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" s="56" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q14" s="57"/>
       <c r="R14" s="57"/>
       <c r="S14" s="57"/>
@@ -10265,7 +10265,7 @@
       <c r="AC14" s="57"/>
       <c r="AD14" s="57"/>
     </row>
-    <row r="15" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
         <v>28</v>
       </c>
@@ -10351,7 +10351,7 @@
       </c>
       <c r="AI15" s="47"/>
     </row>
-    <row r="16" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C16" s="15" t="s">
         <v>101</v>
       </c>
@@ -10413,7 +10413,7 @@
       </c>
       <c r="AI16" s="47"/>
     </row>
-    <row r="17" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="S17" s="16"/>
@@ -10442,7 +10442,7 @@
       <c r="AD17" s="50"/>
       <c r="AI17" s="47"/>
     </row>
-    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="15" t="s">
         <v>200</v>
       </c>
@@ -10492,7 +10492,7 @@
       <c r="AD18" s="50"/>
       <c r="AI18" s="47"/>
     </row>
-    <row r="19" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="V19" s="47"/>
       <c r="W19" s="15" t="s">
         <v>38</v>
@@ -10510,7 +10510,7 @@
       <c r="AD19" s="50"/>
       <c r="AI19" s="47"/>
     </row>
-    <row r="20" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="C20"/>
@@ -10552,7 +10552,7 @@
       <c r="AH20"/>
       <c r="AI20" s="47"/>
     </row>
-    <row r="21" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="C21" s="15" t="s">
@@ -10606,7 +10606,7 @@
       <c r="AH21"/>
       <c r="AI21" s="47"/>
     </row>
-    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
       <c r="S22" s="16"/>
@@ -10622,7 +10622,7 @@
       <c r="AD22" s="50"/>
       <c r="AI22" s="47"/>
     </row>
-    <row r="23" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C23" s="15" t="s">
         <v>116</v>
       </c>
@@ -10698,7 +10698,7 @@
       </c>
       <c r="AI23" s="47"/>
     </row>
-    <row r="24" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
       <c r="S24" s="16"/>
@@ -10736,7 +10736,7 @@
       </c>
       <c r="AI24" s="47"/>
     </row>
-    <row r="25" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
       <c r="S25" s="16"/>
@@ -10752,7 +10752,7 @@
       <c r="AD25" s="50"/>
       <c r="AI25" s="47"/>
     </row>
-    <row r="26" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
       <c r="S26" s="16"/>
@@ -10768,7 +10768,7 @@
       <c r="AD26" s="50"/>
       <c r="AI26" s="47"/>
     </row>
-    <row r="27" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
       <c r="S27" s="16"/>
@@ -10784,7 +10784,7 @@
       <c r="AD27" s="50"/>
       <c r="AI27" s="47"/>
     </row>
-    <row r="28" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="S28" s="16"/>
@@ -10800,7 +10800,7 @@
       <c r="AD28" s="50"/>
       <c r="AI28" s="47"/>
     </row>
-    <row r="29" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:35" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
       <c r="S29" s="16"/>
@@ -10816,42 +10816,42 @@
       <c r="AD29" s="50"/>
       <c r="AI29" s="47"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
     </row>
   </sheetData>
   <conditionalFormatting sqref="AE9:XFD10 W11 AI15:XFD21 F29:XFD29 E9:V9 N30:XFD31 M29:M31 E22:XFD28 E18:V18 E21:AH21 E16:AH17 E30:E31 G30:L31 E12:XFD14 E4:XFD8 A10:B10 A21:C31 A12:C18 A4:C9 A19:B19">
-    <cfRule type="cellIs" dxfId="20" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="7" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W9:AD10">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AE18:AH19 W20 E15:F15 Q15:AH15 H15:M15">
-    <cfRule type="cellIs" dxfId="18" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W18:AD19">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N15:P15">
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G15">
-    <cfRule type="cellIs" dxfId="14" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"nil"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10868,14 +10868,14 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>123</v>
       </c>
@@ -10901,7 +10901,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>126</v>
       </c>
@@ -10921,7 +10921,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
         <v>195</v>
       </c>
@@ -10932,7 +10932,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C5" t="s">
         <v>197</v>
       </c>
@@ -10949,7 +10949,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D6">
         <v>1</v>
       </c>
@@ -10960,7 +10960,7 @@
         <v>50000</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D7">
         <v>4</v>
       </c>
@@ -10971,7 +10971,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D8">
         <v>52</v>
       </c>
@@ -10983,7 +10983,7 @@
         <v>7000</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="D9">
         <v>208</v>
       </c>
@@ -10994,7 +10994,7 @@
         <v>3500</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>123</v>
       </c>
@@ -11014,7 +11014,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>126</v>
       </c>
@@ -11037,7 +11037,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C14" t="s">
         <v>195</v>
       </c>
@@ -11051,7 +11051,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C15" t="s">
         <v>113</v>
       </c>
@@ -11065,7 +11065,7 @@
         <v>30000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C16" t="s">
         <v>112</v>
       </c>
@@ -11092,14 +11092,14 @@
       <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="59.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="59.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -11107,7 +11107,7 @@
       <c r="C2" s="5"/>
       <c r="D2" s="5"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="40" t="s">
         <v>6</v>
       </c>
@@ -11119,7 +11119,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>209</v>
       </c>
@@ -11133,7 +11133,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
         <v>209</v>
       </c>
@@ -11147,7 +11147,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
         <v>209</v>
       </c>
@@ -11161,7 +11161,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
         <v>209</v>
       </c>
@@ -11175,7 +11175,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>209</v>
       </c>
@@ -11189,7 +11189,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
         <v>209</v>
       </c>
@@ -11203,7 +11203,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
         <v>209</v>
       </c>
@@ -11217,7 +11217,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
         <v>209</v>
       </c>
@@ -11231,7 +11231,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
         <v>209</v>
       </c>
@@ -11245,7 +11245,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
         <v>209</v>
       </c>
@@ -11259,7 +11259,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
         <v>209</v>
       </c>
@@ -11273,7 +11273,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>209</v>
       </c>
@@ -11287,7 +11287,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
         <v>209</v>
       </c>
@@ -11301,7 +11301,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="33" t="s">
         <v>224</v>
       </c>
@@ -11315,7 +11315,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="33" t="s">
         <v>224</v>
       </c>
@@ -11329,7 +11329,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
         <v>209</v>
       </c>
@@ -11343,7 +11343,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="32"/>
       <c r="B20" s="32"/>
       <c r="C20" s="32" t="e">
@@ -11351,7 +11351,7 @@
       </c>
       <c r="D20" s="32"/>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="35"/>
       <c r="B21" s="35"/>
       <c r="C21" s="35" t="e">
@@ -11359,7 +11359,7 @@
       </c>
       <c r="D21" s="35"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>227</v>
       </c>
@@ -11373,7 +11373,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="33" t="s">
         <v>227</v>
       </c>
@@ -11387,7 +11387,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="32" t="s">
         <v>227</v>
       </c>
@@ -11401,7 +11401,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="33" t="s">
         <v>227</v>
       </c>
@@ -11415,7 +11415,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="32" t="s">
         <v>227</v>
       </c>
@@ -11429,7 +11429,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="35"/>
       <c r="B27" s="35"/>
       <c r="C27" s="35" t="e">
@@ -11437,7 +11437,7 @@
       </c>
       <c r="D27" s="35"/>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="32" t="s">
         <v>234</v>
       </c>
@@ -11451,7 +11451,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="33" t="s">
         <v>234</v>
       </c>
@@ -11465,7 +11465,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="32" t="s">
         <v>234</v>
       </c>
@@ -11479,7 +11479,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="33" t="s">
         <v>238</v>
       </c>
@@ -11493,7 +11493,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="32" t="s">
         <v>238</v>
       </c>
@@ -11507,7 +11507,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="33" t="s">
         <v>239</v>
       </c>
@@ -11521,7 +11521,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="35"/>
       <c r="B34" s="35"/>
       <c r="C34" s="35" t="e">
@@ -11529,7 +11529,7 @@
       </c>
       <c r="D34" s="35"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="33" t="s">
         <v>241</v>
       </c>
@@ -11543,7 +11543,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="32" t="s">
         <v>241</v>
       </c>
@@ -11557,7 +11557,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="33" t="s">
         <v>241</v>
       </c>
@@ -11571,7 +11571,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="32" t="s">
         <v>245</v>
       </c>
@@ -11585,7 +11585,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" s="33" t="s">
         <v>245</v>
       </c>
@@ -11599,7 +11599,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="37"/>
       <c r="B40" s="37"/>
       <c r="C40" s="37" t="e">
@@ -11607,7 +11607,7 @@
       </c>
       <c r="D40" s="38"/>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="35"/>
       <c r="B41" s="35"/>
       <c r="C41" s="35" t="e">
@@ -11615,7 +11615,7 @@
       </c>
       <c r="D41" s="35"/>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="32" t="s">
         <v>246</v>
       </c>
@@ -11629,7 +11629,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" s="35"/>
       <c r="B43" s="35"/>
       <c r="C43" s="35" t="e">
@@ -11637,7 +11637,7 @@
       </c>
       <c r="D43" s="35"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="32" t="s">
         <v>247</v>
       </c>
@@ -11651,7 +11651,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" s="33" t="s">
         <v>247</v>
       </c>
@@ -11665,7 +11665,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" s="32" t="s">
         <v>249</v>
       </c>
@@ -11679,7 +11679,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="33" t="s">
         <v>249</v>
       </c>
@@ -11693,7 +11693,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A48" s="32" t="s">
         <v>249</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="33" t="s">
         <v>252</v>
       </c>
@@ -11721,7 +11721,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A50" s="32" t="s">
         <v>252</v>
       </c>
@@ -11735,7 +11735,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A51" s="33" t="s">
         <v>252</v>
       </c>
@@ -11749,7 +11749,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A52" s="32" t="s">
         <v>252</v>
       </c>
@@ -11763,7 +11763,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="33" t="s">
         <v>252</v>
       </c>
@@ -11777,7 +11777,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="32" t="s">
         <v>254</v>
       </c>
@@ -11791,7 +11791,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="33" t="s">
         <v>254</v>
       </c>
@@ -11805,7 +11805,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="32" t="s">
         <v>254</v>
       </c>
@@ -11819,7 +11819,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="33" t="s">
         <v>254</v>
       </c>
@@ -11833,7 +11833,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="32" t="s">
         <v>255</v>
       </c>
@@ -11847,7 +11847,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="33" t="s">
         <v>255</v>
       </c>
@@ -11861,7 +11861,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="35"/>
       <c r="B60" s="35"/>
       <c r="C60" s="35" t="e">
@@ -11869,7 +11869,7 @@
       </c>
       <c r="D60" s="35"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="33" t="s">
         <v>256</v>
       </c>
@@ -11883,7 +11883,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="32" t="s">
         <v>256</v>
       </c>
@@ -11897,7 +11897,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="33" t="s">
         <v>257</v>
       </c>
@@ -11911,7 +11911,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="32" t="s">
         <v>257</v>
       </c>
@@ -11925,7 +11925,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="33" t="s">
         <v>257</v>
       </c>
@@ -11939,7 +11939,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="32" t="s">
         <v>257</v>
       </c>
@@ -11953,7 +11953,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="37"/>
       <c r="B67" s="37"/>
       <c r="C67" s="37" t="e">
@@ -11961,7 +11961,7 @@
       </c>
       <c r="D67" s="38"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="35"/>
       <c r="B68" s="35"/>
       <c r="C68" s="35" t="e">
@@ -11969,7 +11969,7 @@
       </c>
       <c r="D68" s="35"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="33" t="s">
         <v>258</v>
       </c>
@@ -11983,7 +11983,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="32" t="s">
         <v>259</v>
       </c>
@@ -11997,7 +11997,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="33" t="s">
         <v>259</v>
       </c>

</xml_diff>